<commit_message>
Division de tareas redes y graficas
</commit_message>
<xml_diff>
--- a/Actividades_semillero_2020.xlsx
+++ b/Actividades_semillero_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="60">
   <si>
     <t>Semana</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Flujo de trabajo sobre la implementación del modelo de racionalidad acotada</t>
   </si>
   <si>
-    <t>Presentación del artículo "Self-Organized Division of Cognitive Labor"</t>
-  </si>
-  <si>
     <t>Enero</t>
   </si>
   <si>
@@ -173,6 +170,42 @@
   </si>
   <si>
     <t>Presentación del artículo "Analyzing Computational Models"</t>
+  </si>
+  <si>
+    <t>Presentación del capítulo 10 del libro "Game Theory Evolving"</t>
+  </si>
+  <si>
+    <t>Nicolás</t>
+  </si>
+  <si>
+    <t>Esteban</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAFICA_PUNTAJE-Promedio-Politica_VS_RONDA </t>
+  </si>
+  <si>
+    <t>ESTEBAN</t>
+  </si>
+  <si>
+    <t>GRAFICA_USO-Politica_VS_RONDA</t>
+  </si>
+  <si>
+    <t>MIGUEL</t>
+  </si>
+  <si>
+    <t>RED REGULAR</t>
+  </si>
+  <si>
+    <t>ALEJANDRO</t>
+  </si>
+  <si>
+    <t>RED SMALL WORLD</t>
+  </si>
+  <si>
+    <t>NICOLÁS</t>
   </si>
 </sst>
 </file>
@@ -615,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -627,7 +660,7 @@
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -641,20 +674,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="13" customFormat="1" ht="12.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="12.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -663,12 +696,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
@@ -677,110 +710,111 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>12</v>
@@ -789,12 +823,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
@@ -803,12 +837,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -817,26 +851,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>6</v>
@@ -847,7 +881,7 @@
     </row>
     <row r="17" spans="1:4" s="13" customFormat="1" ht="12.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -858,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>3</v>
@@ -872,10 +906,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>11</v>
@@ -886,10 +920,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>8</v>
@@ -900,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>6</v>
@@ -914,10 +948,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
@@ -928,10 +962,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -942,10 +976,10 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
@@ -956,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>6</v>
@@ -970,13 +1004,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -984,13 +1018,13 @@
         <v>10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,13 +1032,13 @@
         <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1012,13 +1046,13 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1026,13 +1060,13 @@
         <v>13</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1049,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1061,25 +1095,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1">
         <f>SUM(E2:E67)</f>
@@ -1094,11 +1128,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E2" s="2">
         <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
       </c>
       <c r="I2" s="14">
         <f>2000000/I1</f>
@@ -1113,11 +1152,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="E3" s="2">
         <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,11 +1172,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="E4" s="2">
         <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,14 +1189,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E5" s="2">
         <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2">
@@ -1173,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="2">
@@ -1188,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="2">
@@ -1203,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="2">
@@ -1218,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="2">
@@ -1233,7 +1287,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="2">
@@ -1248,7 +1302,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="2">
@@ -1263,7 +1317,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="2">
@@ -1278,7 +1332,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="2">
@@ -1293,7 +1347,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="2">
@@ -1308,7 +1362,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="2">
@@ -1323,7 +1377,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="2">
@@ -1338,7 +1392,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="2">
@@ -1353,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="2">
@@ -1368,7 +1422,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="2">
@@ -1383,7 +1437,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="2">
@@ -1398,7 +1452,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="2">
@@ -1413,7 +1467,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="2">
@@ -1428,7 +1482,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="2">
@@ -1443,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="2">
@@ -1458,7 +1512,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="2">
@@ -1473,7 +1527,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="2">
@@ -1488,7 +1542,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="2">
@@ -1503,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="2">
@@ -1518,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="2">
@@ -1533,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="2">
@@ -1548,7 +1602,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="2">
@@ -1563,7 +1617,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="2">
@@ -1578,7 +1632,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="2">
@@ -1593,7 +1647,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="2">
@@ -1608,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="2">
@@ -1623,7 +1677,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="2">
@@ -1638,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="2">
@@ -1653,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="2">
@@ -1668,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="2">
@@ -1683,7 +1737,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="2">
@@ -1698,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="2">
@@ -1713,7 +1767,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="2">
@@ -1728,7 +1782,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -1742,7 +1796,7 @@
         <v>3</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -1756,7 +1810,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E46" s="2">
         <v>2</v>
@@ -1770,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
@@ -1784,7 +1838,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
@@ -1798,7 +1852,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E49" s="2">
         <v>2</v>
@@ -1812,7 +1866,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E50" s="2">
         <v>2</v>
@@ -1826,7 +1880,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E51" s="2">
         <v>2</v>
@@ -1840,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E52" s="2">
         <v>2</v>
@@ -1854,7 +1908,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E53" s="2">
         <v>2</v>
@@ -1868,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E54" s="2">
         <v>2</v>
@@ -1882,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E55" s="2">
         <v>2</v>
@@ -1896,7 +1950,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E56" s="2">
         <v>2</v>
@@ -1910,7 +1964,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E57" s="2">
         <v>2</v>
@@ -1924,7 +1978,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E58" s="2">
         <v>2</v>
@@ -1938,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E59" s="2">
         <v>2</v>
@@ -1952,7 +2006,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E60" s="2">
         <v>2</v>
@@ -1966,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E61" s="2">
         <v>2</v>
@@ -1980,7 +2034,7 @@
         <v>10</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E62" s="2">
         <v>2</v>
@@ -1994,7 +2048,7 @@
         <v>10</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E63" s="2">
         <v>2</v>
@@ -2008,7 +2062,7 @@
         <v>10</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E64" s="2">
         <v>2</v>
@@ -2022,7 +2076,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E65" s="2">
         <v>2</v>
@@ -2036,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -2050,7 +2104,7 @@
         <v>11</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E67" s="2">
         <v>2</v>

</xml_diff>